<commit_message>
Chỉnh sửa lỗi code và lỗi dữ liệu trong file excel
</commit_message>
<xml_diff>
--- a/netbox_create_data/file_data/netbox_info.xlsx
+++ b/netbox_create_data/file_data/netbox_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NetBox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6259B49-85CA-4E3C-A73F-FED79214C077}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF83DE5-1922-4D61-A2FB-8FC4DB942EB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4035" windowWidth="19440" windowHeight="15150" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43515" yWindow="1620" windowWidth="14085" windowHeight="9075" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thong Tin Thiet Bi" sheetId="13" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="270">
   <si>
     <t>active</t>
   </si>
@@ -294,12 +294,6 @@
   </si>
   <si>
     <t>Fiber Patch Panel</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>SW1</t>
   </si>
   <si>
     <t>DNS server 1</t>
@@ -870,6 +864,15 @@
   </si>
   <si>
     <t>ge1/0/4</t>
+  </si>
+  <si>
+    <t>te1/0/1</t>
+  </si>
+  <si>
+    <t>te1/0/2</t>
+  </si>
+  <si>
+    <t>te1/0/3</t>
   </si>
 </sst>
 </file>
@@ -1225,30 +1228,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1275,6 +1254,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1519,37 +1522,37 @@
     <row r="1" spans="2:16" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="G2" s="57" t="s">
         <v>163</v>
-      </c>
-      <c r="F2" s="65" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" s="65" t="s">
-        <v>165</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>77</v>
@@ -1577,16 +1580,16 @@
         <v>83</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>81</v>
@@ -1601,7 +1604,7 @@
         <v>12</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M4" s="3"/>
     </row>
@@ -1613,16 +1616,16 @@
         <v>79</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>82</v>
@@ -1637,7 +1640,7 @@
         <v>13</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M5" s="3"/>
     </row>
@@ -1649,16 +1652,16 @@
         <v>80</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>82</v>
@@ -1673,7 +1676,7 @@
         <v>14</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -1682,19 +1685,19 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>82</v>
@@ -1709,7 +1712,7 @@
         <v>15</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M7" s="3"/>
     </row>
@@ -1721,16 +1724,16 @@
         <v>78</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>26</v>
@@ -1745,7 +1748,7 @@
         <v>12</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M8" s="3"/>
       <c r="P8" s="46"/>
@@ -1758,16 +1761,16 @@
         <v>53</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>20</v>
@@ -1782,7 +1785,7 @@
         <v>13</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M9" s="3"/>
       <c r="P9" s="46"/>
@@ -1795,16 +1798,16 @@
         <v>84</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>20</v>
@@ -1819,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M10" s="3"/>
       <c r="P10" s="46"/>
@@ -1832,16 +1835,16 @@
         <v>54</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>27</v>
@@ -1856,7 +1859,7 @@
         <v>7</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="47"/>
@@ -1869,16 +1872,16 @@
         <v>52</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>28</v>
@@ -1893,7 +1896,7 @@
         <v>9</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M12" s="3"/>
     </row>
@@ -1928,9 +1931,9 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="69" t="s">
-        <v>166</v>
+      <c r="K18" s="58"/>
+      <c r="L18" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="3:13" ht="13.8" x14ac:dyDescent="0.25">
@@ -1941,9 +1944,9 @@
       <c r="G19" s="11"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="69" t="s">
-        <v>167</v>
+      <c r="K19" s="59"/>
+      <c r="L19" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="3:13" ht="13.8" x14ac:dyDescent="0.25">
@@ -1954,9 +1957,9 @@
       <c r="G20" s="11"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="69" t="s">
-        <v>168</v>
+      <c r="K20" s="60"/>
+      <c r="L20" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
@@ -1977,7 +1980,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="48"/>
+      <c r="I22" s="68"/>
       <c r="J22" s="10"/>
       <c r="M22" s="10"/>
     </row>
@@ -1987,8 +1990,8 @@
       <c r="E23" s="13"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="48"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="68"/>
       <c r="J23" s="10"/>
       <c r="M23" s="10"/>
     </row>
@@ -1998,8 +2001,8 @@
       <c r="E24" s="13"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
       <c r="J24" s="10"/>
       <c r="K24" s="14"/>
       <c r="L24" s="19"/>
@@ -2135,25 +2138,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
-        <v>180</v>
+      <c r="A1" s="62" t="s">
+        <v>178</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>117</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>119</v>
       </c>
       <c r="C2" s="18">
         <v>630</v>
@@ -2163,11 +2166,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="67" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C3" s="43">
         <v>631</v>
@@ -2177,11 +2180,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="67" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="43">
         <v>632</v>
@@ -2191,11 +2194,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="67" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" s="43">
         <v>633</v>
@@ -2205,11 +2208,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="67" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" s="18">
         <v>634</v>
@@ -2219,11 +2222,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="67" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" s="18">
         <v>635</v>
@@ -2258,25 +2261,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>180</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>182</v>
       </c>
       <c r="D1" s="41" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>183</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>184</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2300,8 +2303,8 @@
       <c r="F2" s="35">
         <v>1232342</v>
       </c>
-      <c r="G2" s="74" t="s">
-        <v>255</v>
+      <c r="G2" s="66" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2325,12 +2328,12 @@
       <c r="F3" s="35">
         <v>134141</v>
       </c>
-      <c r="G3" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="69" t="s">
-        <v>166</v>
+      <c r="G3" s="66" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="58"/>
+      <c r="J3" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2354,12 +2357,12 @@
       <c r="F4" s="35">
         <v>1313114</v>
       </c>
-      <c r="G4" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="69" t="s">
-        <v>167</v>
+      <c r="G4" s="66" t="s">
+        <v>255</v>
+      </c>
+      <c r="I4" s="59"/>
+      <c r="J4" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2383,12 +2386,12 @@
       <c r="F5" s="35">
         <v>24241414</v>
       </c>
-      <c r="G5" s="74" t="s">
-        <v>258</v>
-      </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69" t="s">
-        <v>168</v>
+      <c r="G5" s="66" t="s">
+        <v>256</v>
+      </c>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2412,8 +2415,8 @@
       <c r="F6" s="35">
         <v>13124141414</v>
       </c>
-      <c r="G6" s="74" t="s">
-        <v>259</v>
+      <c r="G6" s="66" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2461,43 +2464,43 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>186</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>188</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H1" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="K1" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="K1" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="L1" s="40" t="s">
-        <v>193</v>
-      </c>
       <c r="M1" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N1" s="33" t="s">
         <v>77</v>
@@ -2540,7 +2543,7 @@
         <v>48</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -2562,7 +2565,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>34</v>
@@ -2580,7 +2583,7 @@
         <v>48</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -2602,7 +2605,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G4" s="35" t="s">
         <v>35</v>
@@ -2620,7 +2623,7 @@
         <v>48</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -2642,7 +2645,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>36</v>
@@ -2660,7 +2663,7 @@
         <v>48</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -2682,13 +2685,13 @@
         <v>24</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I6" s="35">
         <v>21</v>
@@ -2700,7 +2703,7 @@
         <v>48</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -2722,13 +2725,13 @@
         <v>24</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I7" s="35">
         <v>21</v>
@@ -2740,25 +2743,25 @@
         <v>48</v>
       </c>
       <c r="N7" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="G13" s="66"/>
-      <c r="H13" s="69" t="s">
+      <c r="G13" s="58"/>
+      <c r="H13" s="61" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="G14" s="59"/>
+      <c r="H14" s="61" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="G15" s="60"/>
+      <c r="H15" s="61" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="G14" s="67"/>
-      <c r="H14" s="69" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="G15" s="68"/>
-      <c r="H15" s="69" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2805,31 +2808,31 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="48" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="66"/>
-      <c r="J1" s="69" t="s">
-        <v>166</v>
+      <c r="I1" s="58"/>
+      <c r="J1" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B2" s="35">
         <v>1</v>
@@ -2846,14 +2849,14 @@
         <f>IF(ISERROR(MATCH('Kieu thiet bi'!A2,interface_templates!A:A,0)),"no", "yes")</f>
         <v>yes</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="69" t="s">
-        <v>167</v>
+      <c r="I2" s="59"/>
+      <c r="J2" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B3" s="35">
         <v>1</v>
@@ -2870,14 +2873,14 @@
         <f>IF(ISERROR(MATCH('Kieu thiet bi'!A3,interface_templates!A:A,0)),"no", "yes")</f>
         <v>yes</v>
       </c>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69" t="s">
-        <v>168</v>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B4" s="35">
         <v>1</v>
@@ -2894,14 +2897,14 @@
         <f>IF(ISERROR(MATCH('Kieu thiet bi'!A4,interface_templates!A:A,0)),"no", "yes")</f>
         <v>yes</v>
       </c>
-      <c r="I4" s="64" t="s">
-        <v>206</v>
+      <c r="I4" s="56" t="s">
+        <v>204</v>
       </c>
       <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B5" s="35">
         <v>1</v>
@@ -2918,21 +2921,21 @@
         <f>IF(ISERROR(MATCH('Kieu thiet bi'!A5,interface_templates!A:A,0)),"no", "yes")</f>
         <v>yes</v>
       </c>
-      <c r="I5" s="58" t="s">
-        <v>226</v>
+      <c r="I5" s="50" t="s">
+        <v>224</v>
       </c>
       <c r="J5" s="47" t="s">
-        <v>229</v>
-      </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
+        <v>227</v>
+      </c>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
     </row>
     <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B6" s="35">
         <v>2</v>
@@ -2949,16 +2952,16 @@
         <f>IF(ISERROR(MATCH('Kieu thiet bi'!A6,interface_templates!A:A,0)),"no", "yes")</f>
         <v>yes</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="65" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="47" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B7" s="35">
         <v>1</v>
@@ -2975,16 +2978,16 @@
         <f>IF(ISERROR(MATCH('Kieu thiet bi'!A7,interface_templates!A:A,0)),"no", "yes")</f>
         <v>yes</v>
       </c>
-      <c r="I7" s="73" t="s">
+      <c r="I7" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="58" t="s">
-        <v>224</v>
+      <c r="J7" s="50" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B8" s="35">
         <v>1</v>
@@ -3004,7 +3007,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B9" s="35">
         <v>2</v>
@@ -3062,37 +3065,37 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B2" s="18" t="str">
         <f>VLOOKUP(A2,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Cisco</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>13</v>
@@ -3103,17 +3106,17 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B3" s="18" t="str">
         <f>VLOOKUP(A3,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Cisco</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>9</v>
@@ -3124,20 +3127,20 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B4" s="18" t="str">
         <f>VLOOKUP(A4,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Cisco</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>6</v>
@@ -3145,17 +3148,17 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" s="18" t="str">
         <f>VLOOKUP(A5,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>13</v>
@@ -3166,20 +3169,20 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B6" s="18" t="str">
         <f>VLOOKUP(A6,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D6" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>238</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>240</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>6</v>
@@ -3187,32 +3190,32 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B7" s="18" t="str">
         <f>VLOOKUP(A7,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D7" s="18">
         <v>1</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="66"/>
-      <c r="I7" s="69" t="s">
-        <v>166</v>
+      <c r="H7" s="58"/>
+      <c r="I7" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B8" s="18" t="str">
         <f>VLOOKUP(A8,'Kieu thiet bi'!A:E,5,0)</f>
@@ -3230,39 +3233,39 @@
       <c r="F8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="67"/>
-      <c r="I8" s="69" t="s">
-        <v>167</v>
+      <c r="H8" s="59"/>
+      <c r="I8" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B9" s="18" t="str">
         <f>VLOOKUP(A9,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="68"/>
-      <c r="I9" s="69" t="s">
-        <v>168</v>
+      <c r="H9" s="60"/>
+      <c r="I9" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B10" s="18" t="str">
         <f>VLOOKUP(A10,'Kieu thiet bi'!A:E,5,0)</f>
@@ -3283,17 +3286,17 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B11" s="18" t="str">
         <f>VLOOKUP(A11,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>13</v>
@@ -3304,95 +3307,95 @@
     </row>
     <row r="12" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B12" s="18" t="str">
         <f>VLOOKUP(A12,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D12" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>238</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>240</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="71" t="s">
-        <v>221</v>
+      <c r="H12" s="63" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B13" s="18" t="str">
         <f>VLOOKUP(A13,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D13" s="18">
         <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="70" t="s">
-        <v>175</v>
+      <c r="H13" s="62" t="s">
+        <v>173</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B14" s="18" t="str">
         <f>VLOOKUP(A14,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Dell</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="70" t="s">
-        <v>177</v>
+      <c r="H14" s="62" t="s">
+        <v>175</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B15" s="18" t="str">
         <f>VLOOKUP(A15,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Dell</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>13</v>
@@ -3403,20 +3406,20 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B16" s="18" t="str">
         <f>VLOOKUP(A16,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Dell</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D16" s="18">
         <v>1</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>6</v>
@@ -3424,17 +3427,17 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B17" s="18" t="str">
         <f>VLOOKUP(A17,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Cisco</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>13</v>
@@ -3445,20 +3448,20 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B18" s="18" t="str">
         <f>VLOOKUP(A18,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Cisco</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>6</v>
@@ -3466,17 +3469,17 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B19" s="18" t="str">
         <f>VLOOKUP(A19,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>13</v>
@@ -3487,20 +3490,20 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B20" s="18" t="str">
         <f>VLOOKUP(A20,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>6</v>
@@ -3508,20 +3511,20 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B21" s="18" t="str">
         <f>VLOOKUP(A21,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Lenovo</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D21" s="18">
         <v>1</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>6</v>
@@ -3529,7 +3532,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22" s="18" t="str">
         <f>VLOOKUP(A22,'Kieu thiet bi'!A:E,5,0)</f>
@@ -3550,17 +3553,17 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B23" s="18" t="str">
         <f>VLOOKUP(A23,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Dell</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>13</v>
@@ -3571,20 +3574,20 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B24" s="18" t="str">
         <f>VLOOKUP(A24,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Dell</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>6</v>
@@ -3592,20 +3595,20 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B25" s="18" t="str">
         <f>VLOOKUP(A25,'Kieu thiet bi'!A:E,5,0)</f>
         <v>Dell</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D25" s="18">
         <v>2</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>6</v>
@@ -3654,7 +3657,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>8</v>
@@ -3699,9 +3702,9 @@
       <c r="B6" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="66"/>
-      <c r="F6" s="69" t="s">
-        <v>166</v>
+      <c r="E6" s="58"/>
+      <c r="F6" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -3711,9 +3714,9 @@
       <c r="B7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="69" t="s">
-        <v>167</v>
+      <c r="E7" s="59"/>
+      <c r="F7" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -3723,9 +3726,9 @@
       <c r="B8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69" t="s">
-        <v>168</v>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -3743,11 +3746,11 @@
       <c r="B10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="65" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -3797,46 +3800,46 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E1" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="61" t="s">
+      <c r="K1" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I1" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="J1" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="K1" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="L1" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>77</v>
@@ -4038,7 +4041,7 @@
         <v>HungNV</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I5" s="18" t="str">
         <f>VLOOKUP(B5,'Thong Tin Thiet Bi'!C:G,4,0)</f>
@@ -4063,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -4094,7 +4097,7 @@
         <v>HaiDD</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I6" s="18" t="str">
         <f>VLOOKUP(B6,'Thong Tin Thiet Bi'!C:G,4,0)</f>
@@ -4119,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -4169,13 +4172,13 @@
         <v>13</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -4206,7 +4209,7 @@
         <v>TanNT</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I8" s="18" t="str">
         <f>VLOOKUP(B8,'Thong Tin Thiet Bi'!C:G,4,0)</f>
@@ -4231,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -4262,7 +4265,7 @@
         <v>LongLQ</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I9" s="18" t="str">
         <f>VLOOKUP(B9,'Thong Tin Thiet Bi'!C:G,4,0)</f>
@@ -4287,7 +4290,7 @@
         <v>12</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -4343,64 +4346,64 @@
         <v>0</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="59"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="59"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="59"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="69" t="s">
-        <v>166</v>
+      <c r="A15" s="51"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M16" s="72"/>
-      <c r="N16" s="69" t="s">
-        <v>167</v>
+      <c r="M16" s="64"/>
+      <c r="N16" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="13:14" x14ac:dyDescent="0.3">
       <c r="M17" s="42"/>
       <c r="N17" s="46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="13:14" x14ac:dyDescent="0.3">
       <c r="M18" s="47"/>
     </row>
     <row r="19" spans="13:14" x14ac:dyDescent="0.3">
-      <c r="M19" s="70" t="s">
-        <v>213</v>
+      <c r="M19" s="62" t="s">
+        <v>211</v>
       </c>
       <c r="N19" s="38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4454,29 +4457,29 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>209</v>
-      </c>
       <c r="D1" s="33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>77</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="55" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="37" t="s">
@@ -4489,7 +4492,7 @@
       <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="55" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="37" t="s">
@@ -4502,7 +4505,7 @@
       <c r="A4" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="55" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="37" t="s">
@@ -4510,16 +4513,16 @@
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="69" t="s">
-        <v>166</v>
+      <c r="H4" s="58"/>
+      <c r="I4" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="55" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="37" t="s">
@@ -4527,26 +4530,26 @@
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="69" t="s">
-        <v>167</v>
+      <c r="H5" s="59"/>
+      <c r="I5" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="35"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69" t="s">
-        <v>168</v>
+      <c r="H6" s="60"/>
+      <c r="I6" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -4562,40 +4565,40 @@
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
       <c r="E8" s="35"/>
-      <c r="H8" s="57" t="s">
-        <v>204</v>
+      <c r="H8" s="49" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H9" s="70" t="s">
-        <v>202</v>
+      <c r="H9" s="62" t="s">
+        <v>200</v>
       </c>
       <c r="I9" s="38" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H10" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="62" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H10" s="70" t="s">
-        <v>203</v>
-      </c>
-      <c r="I10" s="38" t="s">
+      <c r="I11" s="38" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H11" s="70" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="I11" s="38" t="s">
+      <c r="I12" s="38" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H12" s="70" t="s">
-        <v>218</v>
-      </c>
-      <c r="I12" s="38" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -4615,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E61F048-B9B3-447E-BB41-6DB2F2DF25B5}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4639,46 +4642,46 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>77</v>
@@ -4693,7 +4696,7 @@
         <v>SW 2</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -4709,36 +4712,36 @@
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="50">
+      <c r="A3" s="72">
         <v>2</v>
       </c>
-      <c r="B3" s="52" t="str">
+      <c r="B3" s="70" t="str">
         <f>VLOOKUP(A3,'Thong Tin Thiet Bi'!B3:C12,2,0)</f>
         <v>DNS server</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F3" s="18">
         <v>24</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>10</v>
@@ -4747,7 +4750,7 @@
         <v>10</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N3" s="30" t="s">
         <v>6</v>
@@ -4755,31 +4758,31 @@
       <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="53"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F4" s="18">
         <v>24</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -4788,7 +4791,7 @@
         <v>12</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N4" s="30" t="s">
         <v>6</v>
@@ -4796,36 +4799,36 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="50">
+      <c r="A5" s="72">
         <v>3</v>
       </c>
-      <c r="B5" s="52" t="str">
+      <c r="B5" s="70" t="str">
         <f>VLOOKUP(A5,'Thong Tin Thiet Bi'!B4:C13,2,0)</f>
         <v>FTP server</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F5" s="18">
         <v>24</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K5" s="20" t="s">
         <v>10</v>
@@ -4834,7 +4837,7 @@
         <v>23</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>6</v>
@@ -4842,40 +4845,40 @@
       <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="18" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>73</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F6" s="18">
         <v>24</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>53</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L6" s="20">
         <v>34</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N6" s="31" t="s">
         <v>6</v>
@@ -4883,31 +4886,31 @@
       <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="53"/>
+      <c r="A7" s="74"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="18" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F7" s="18">
         <v>24</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>10</v>
@@ -4916,7 +4919,7 @@
         <v>54</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N7" s="31" t="s">
         <v>6</v>
@@ -4932,37 +4935,37 @@
         <v>DNS server 1</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F8" s="18">
         <v>24</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>83</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L8" s="18">
         <v>21</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N8" s="30" t="s">
         <v>6</v>
@@ -4970,36 +4973,36 @@
       <c r="O8" s="18"/>
     </row>
     <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="50">
+      <c r="A9" s="72">
         <v>5</v>
       </c>
-      <c r="B9" s="52" t="str">
+      <c r="B9" s="70" t="str">
         <f>VLOOKUP(A9,'Thong Tin Thiet Bi'!B6:C15,2,0)</f>
         <v>Openstack server</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F9" s="18">
         <v>24</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>53</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>10</v>
@@ -5008,7 +5011,7 @@
         <v>21</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N9" s="30" t="s">
         <v>6</v>
@@ -5016,40 +5019,40 @@
       <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="55"/>
-      <c r="B10" s="54"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F10" s="18">
         <v>24</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>83</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L10" s="18">
         <v>13</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N10" s="30" t="s">
         <v>6</v>
@@ -5057,31 +5060,31 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="55"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F11" s="18">
         <v>24</v>
       </c>
       <c r="G11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>118</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>53</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>10</v>
@@ -5090,7 +5093,7 @@
         <v>17</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N11" s="30" t="s">
         <v>6</v>
@@ -5098,31 +5101,31 @@
       <c r="O11" s="18"/>
     </row>
     <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F12" s="18">
         <v>24</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>53</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K12" s="18" t="s">
         <v>10</v>
@@ -5131,7 +5134,7 @@
         <v>21</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N12" s="30" t="s">
         <v>6</v>
@@ -5147,7 +5150,7 @@
         <v>SW 1</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -5163,36 +5166,36 @@
       <c r="O13" s="18"/>
     </row>
     <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="52">
+      <c r="A14" s="70">
         <v>7</v>
       </c>
-      <c r="B14" s="52" t="str">
+      <c r="B14" s="70" t="str">
         <f>VLOOKUP(A14,'Thong Tin Thiet Bi'!B8:C17,2,0)</f>
         <v>DHCP server</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="F14" s="52">
+        <v>258</v>
+      </c>
+      <c r="D14" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="70">
         <v>24</v>
       </c>
-      <c r="G14" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="H14" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="I14" s="52" t="s">
+      <c r="G14" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="70" t="s">
         <v>53</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K14" s="27" t="s">
         <v>10</v>
@@ -5201,7 +5204,7 @@
         <v>14</v>
       </c>
       <c r="M14" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N14" s="32" t="s">
         <v>5</v>
@@ -5209,19 +5212,19 @@
       <c r="O14" s="18"/>
     </row>
     <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
+        <v>260</v>
+      </c>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
       <c r="J15" s="27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K15" s="27" t="s">
         <v>10</v>
@@ -5230,15 +5233,15 @@
         <v>16</v>
       </c>
       <c r="M15" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N15" s="32" t="s">
         <v>6</v>
       </c>
       <c r="O15" s="18"/>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="69" t="s">
-        <v>166</v>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -5250,28 +5253,28 @@
         <v>APP Server</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F16" s="18">
         <v>24</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>83</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K16" s="18" t="s">
         <v>10</v>
@@ -5280,15 +5283,15 @@
         <v>13</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="N16" s="30" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="18"/>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="69" t="s">
-        <v>167</v>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="61" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -5300,28 +5303,28 @@
         <v>DB Server</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F17" s="18">
         <v>24</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>53</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K17" s="18" t="s">
         <v>10</v>
@@ -5330,19 +5333,24 @@
         <v>12</v>
       </c>
       <c r="M17" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N17" s="30" t="s">
         <v>6</v>
       </c>
       <c r="O17" s="18"/>
-      <c r="P17" s="68"/>
-      <c r="Q17" s="69" t="s">
-        <v>168</v>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="A9:A12"/>
@@ -5352,11 +5360,6 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
thêm tính năng add lag(bond) cho interface
</commit_message>
<xml_diff>
--- a/netbox_create_data/file_data/netbox_info.xlsx
+++ b/netbox_create_data/file_data/netbox_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NetBox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF83DE5-1922-4D61-A2FB-8FC4DB942EB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8C57BC-7DDA-48FE-93F6-C6FC36044A0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43515" yWindow="1620" windowWidth="14085" windowHeight="9075" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thong Tin Thiet Bi" sheetId="13" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="270">
   <si>
     <t>active</t>
   </si>
@@ -1115,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1261,22 +1261,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4618,8 +4621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E61F048-B9B3-447E-BB41-6DB2F2DF25B5}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4632,7 +4635,7 @@
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
     <col min="10" max="11" width="14.77734375" customWidth="1"/>
     <col min="12" max="12" width="10.44140625" customWidth="1"/>
     <col min="13" max="13" width="13.88671875" customWidth="1"/>
@@ -4698,7 +4701,9 @@
       <c r="C2" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="25"/>
+      <c r="D2" s="25" t="s">
+        <v>146</v>
+      </c>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
@@ -4712,10 +4717,10 @@
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="72">
+      <c r="A3" s="70">
         <v>2</v>
       </c>
-      <c r="B3" s="70" t="str">
+      <c r="B3" s="72" t="str">
         <f>VLOOKUP(A3,'Thong Tin Thiet Bi'!B3:C12,2,0)</f>
         <v>DNS server</v>
       </c>
@@ -4758,8 +4763,8 @@
       <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
-      <c r="B4" s="71"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="18" t="s">
         <v>259</v>
       </c>
@@ -4799,10 +4804,10 @@
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="72">
+      <c r="A5" s="70">
         <v>3</v>
       </c>
-      <c r="B5" s="70" t="str">
+      <c r="B5" s="72" t="str">
         <f>VLOOKUP(A5,'Thong Tin Thiet Bi'!B4:C13,2,0)</f>
         <v>FTP server</v>
       </c>
@@ -4845,8 +4850,8 @@
       <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="73"/>
-      <c r="B6" s="75"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="18" t="s">
         <v>268</v>
       </c>
@@ -4886,8 +4891,8 @@
       <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="74"/>
-      <c r="B7" s="71"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="73"/>
       <c r="C7" s="18" t="s">
         <v>269</v>
       </c>
@@ -4973,10 +4978,10 @@
       <c r="O8" s="18"/>
     </row>
     <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="72">
+      <c r="A9" s="70">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="str">
+      <c r="B9" s="72" t="str">
         <f>VLOOKUP(A9,'Thong Tin Thiet Bi'!B6:C15,2,0)</f>
         <v>Openstack server</v>
       </c>
@@ -5019,8 +5024,8 @@
       <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="73"/>
-      <c r="B10" s="75"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="18" t="s">
         <v>260</v>
       </c>
@@ -5060,8 +5065,8 @@
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="73"/>
-      <c r="B11" s="75"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="18" t="s">
         <v>261</v>
       </c>
@@ -5101,8 +5106,8 @@
       <c r="O11" s="18"/>
     </row>
     <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="18" t="s">
         <v>259</v>
       </c>
@@ -5152,7 +5157,9 @@
       <c r="C13" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="76" t="s">
+        <v>146</v>
+      </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
@@ -5166,32 +5173,32 @@
       <c r="O13" s="18"/>
     </row>
     <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="70">
+      <c r="A14" s="72">
         <v>7</v>
       </c>
-      <c r="B14" s="70" t="str">
+      <c r="B14" s="72" t="str">
         <f>VLOOKUP(A14,'Thong Tin Thiet Bi'!B8:C17,2,0)</f>
         <v>DHCP server</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="D14" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="70">
+      <c r="F14" s="72">
         <v>24</v>
       </c>
-      <c r="G14" s="70" t="s">
+      <c r="G14" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="H14" s="70" t="s">
+      <c r="H14" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="I14" s="70" t="s">
+      <c r="I14" s="72" t="s">
         <v>53</v>
       </c>
       <c r="J14" s="27" t="s">
@@ -5212,17 +5219,17 @@
       <c r="O14" s="18"/>
     </row>
     <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
       <c r="J15" s="27" t="s">
         <v>263</v>
       </c>
@@ -5346,11 +5353,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="A9:A12"/>
@@ -5360,6 +5362,11 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
@@ -5374,13 +5381,19 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C7AF243D-1C79-45FE-A5DD-72B81483D019}">
           <x14:formula1>
             <xm:f>'Region va Site'!$B:$B</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{518AA467-C236-4D48-8D09-15319AA5B54C}">
+          <x14:formula1>
+            <xm:f>'Thong Tin Thiet Bi'!$C:$C</xm:f>
+          </x14:formula1>
+          <xm:sqref>I1:I1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
update netbox web service
</commit_message>
<xml_diff>
--- a/netbox_create_data/file_data/netbox_info.xlsx
+++ b/netbox_create_data/file_data/netbox_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NetBox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B1C6A1-CD77-4E99-BA4E-68AE5F125007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9E6764-AA0E-4879-A15F-140D98207B82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4035" windowWidth="19440" windowHeight="15150" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="4035" windowWidth="19440" windowHeight="15150" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dac ta thiet bi" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="344">
   <si>
     <t>active</t>
   </si>
@@ -998,9 +998,6 @@
   </si>
   <si>
     <t>grafana</t>
-  </si>
-  <si>
-    <t>Tên VM</t>
   </si>
   <si>
     <t>IP</t>
@@ -2658,13 +2655,13 @@
         <v>269</v>
       </c>
       <c r="B1" s="78" t="s">
+        <v>333</v>
+      </c>
+      <c r="C1" s="78" t="s">
         <v>334</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="D1" s="78" t="s">
         <v>335</v>
-      </c>
-      <c r="D1" s="78" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -2672,7 +2669,7 @@
         <v>296</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C2" s="79" t="s">
         <v>143</v>
@@ -2709,7 +2706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41472720-35A2-493E-9253-72E72F21EBB8}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2726,19 +2723,19 @@
         <v>30</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="C1" s="84" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="84" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E1" s="84" t="s">
         <v>36</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -2746,13 +2743,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="85" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="86" t="s">
         <v>312</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="D2" s="86" t="s">
         <v>313</v>
-      </c>
-      <c r="D2" s="86" t="s">
-        <v>314</v>
       </c>
       <c r="E2" s="86">
         <v>24</v>
@@ -2765,10 +2762,10 @@
       <c r="A3" s="85"/>
       <c r="B3" s="85"/>
       <c r="C3" s="86" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" s="86" t="s">
         <v>315</v>
-      </c>
-      <c r="D3" s="86" t="s">
-        <v>316</v>
       </c>
       <c r="E3" s="86">
         <v>24</v>
@@ -2781,10 +2778,10 @@
       <c r="A4" s="85"/>
       <c r="B4" s="85"/>
       <c r="C4" s="86" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="86" t="s">
         <v>317</v>
-      </c>
-      <c r="D4" s="86" t="s">
-        <v>318</v>
       </c>
       <c r="E4" s="86">
         <v>24</v>
@@ -2798,13 +2795,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="86" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="D5" s="86" t="s">
         <v>320</v>
-      </c>
-      <c r="D5" s="86" t="s">
-        <v>321</v>
       </c>
       <c r="E5" s="86">
         <v>24</v>
@@ -2818,13 +2815,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="87" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="D6" s="86" t="s">
         <v>322</v>
-      </c>
-      <c r="C6" s="86" t="s">
-        <v>313</v>
-      </c>
-      <c r="D6" s="86" t="s">
-        <v>323</v>
       </c>
       <c r="E6" s="86">
         <v>24</v>
@@ -2837,10 +2834,10 @@
       <c r="A7" s="88"/>
       <c r="B7" s="88"/>
       <c r="C7" s="86" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D7" s="86" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E7" s="86">
         <v>24</v>
@@ -2853,10 +2850,10 @@
       <c r="A8" s="89"/>
       <c r="B8" s="89"/>
       <c r="C8" s="86" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D8" s="86" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E8" s="86">
         <v>24</v>
@@ -2870,13 +2867,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="86" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="D9" s="86" t="s">
         <v>326</v>
-      </c>
-      <c r="C9" s="86" t="s">
-        <v>313</v>
-      </c>
-      <c r="D9" s="86" t="s">
-        <v>327</v>
       </c>
       <c r="E9" s="86">
         <v>24</v>
@@ -2890,13 +2887,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="87" t="s">
+        <v>327</v>
+      </c>
+      <c r="C10" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="D10" s="86" t="s">
         <v>328</v>
-      </c>
-      <c r="C10" s="86" t="s">
-        <v>313</v>
-      </c>
-      <c r="D10" s="86" t="s">
-        <v>329</v>
       </c>
       <c r="E10" s="86">
         <v>24</v>
@@ -2909,10 +2906,10 @@
       <c r="A11" s="88"/>
       <c r="B11" s="88"/>
       <c r="C11" s="86" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D11" s="86" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E11" s="86">
         <v>24</v>
@@ -2925,10 +2922,10 @@
       <c r="A12" s="89"/>
       <c r="B12" s="89"/>
       <c r="C12" s="86" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E12" s="86">
         <v>24</v>
@@ -2942,13 +2939,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="86" t="s">
+        <v>331</v>
+      </c>
+      <c r="C13" s="86" t="s">
+        <v>319</v>
+      </c>
+      <c r="D13" s="86" t="s">
         <v>332</v>
-      </c>
-      <c r="C13" s="86" t="s">
-        <v>320</v>
-      </c>
-      <c r="D13" s="86" t="s">
-        <v>333</v>
       </c>
       <c r="E13" s="86">
         <v>24</v>
@@ -2986,8 +2983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CEE393-B4C5-4266-91B9-AA7C509A519E}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3034,10 +3031,10 @@
         <v>295</v>
       </c>
       <c r="L1" s="80" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M1" s="80" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N1" s="81"/>
       <c r="O1" s="81"/>
@@ -3079,7 +3076,7 @@
         <v>9000</v>
       </c>
       <c r="L2" s="82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M2" s="82" t="s">
         <v>0</v>
@@ -3126,7 +3123,7 @@
         <v>80</v>
       </c>
       <c r="L3" s="82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M3" s="82" t="s">
         <v>0</v>
@@ -3173,7 +3170,7 @@
         <v>443</v>
       </c>
       <c r="L4" s="82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M4" s="82" t="s">
         <v>0</v>
@@ -3220,7 +3217,7 @@
         <v>5044</v>
       </c>
       <c r="L5" s="82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M5" s="82" t="s">
         <v>0</v>
@@ -3304,7 +3301,7 @@
         <v>3030</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M7" s="82" t="s">
         <v>0</v>
@@ -3364,27 +3361,27 @@
     </row>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="79" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>